<commit_message>
fix 2018 dataset and new 2020 dataset for wt v age
also change fledge date plot to average dates per nestbox.
</commit_message>
<xml_diff>
--- a/020_data/2019_PA_chicks.xlsx
+++ b/020_data/2019_PA_chicks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Hanks-Research/2020_Kestrel_Plots/020_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BAF427-2997-2147-9134-5AB572608195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A017439-D8C1-5540-BF00-5F9F6765443B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="460" windowWidth="23260" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -636,8 +636,8 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="8" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D136" sqref="D136"/>
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1275,6 +1275,9 @@
       <c r="E33">
         <v>5</v>
       </c>
+      <c r="I33" s="1">
+        <v>43624</v>
+      </c>
       <c r="J33" t="s">
         <v>65</v>
       </c>
@@ -2443,6 +2446,9 @@
       <c r="E96">
         <v>3</v>
       </c>
+      <c r="I96" s="1">
+        <v>43661</v>
+      </c>
     </row>
     <row r="97" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
@@ -2456,6 +2462,9 @@
       </c>
       <c r="E97">
         <v>4</v>
+      </c>
+      <c r="I97" s="1">
+        <v>43679</v>
       </c>
     </row>
     <row r="98" spans="2:13" x14ac:dyDescent="0.2">

</xml_diff>